<commit_message>
Add MeetingMinute 05/05/2019' '
</commit_message>
<xml_diff>
--- a/MeetingMinutes/PiggyBank.xlsx
+++ b/MeetingMinutes/PiggyBank.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Bảng bỏ heo đi muộn</t>
   </si>
@@ -90,6 +90,15 @@
   </si>
   <si>
     <t>23-04</t>
+  </si>
+  <si>
+    <t>28-04</t>
+  </si>
+  <si>
+    <t>30-04</t>
+  </si>
+  <si>
+    <t>05-05</t>
   </si>
 </sst>
 </file>
@@ -137,7 +146,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -162,6 +171,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -175,7 +190,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -215,6 +230,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -496,7 +514,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:E1"/>
@@ -684,36 +702,62 @@
       <c r="E18" s="9"/>
     </row>
     <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="9"/>
+      <c r="A19" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="11"/>
       <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
+      <c r="D19" s="11"/>
       <c r="E19" s="9"/>
     </row>
     <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="11"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="9"/>
+    </row>
+    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="10">
+        <v>1</v>
+      </c>
+      <c r="C21" s="9"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="9"/>
+    </row>
+    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+    </row>
+    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="6">
-        <f>10 * SUM(B4:B19)</f>
-        <v>30</v>
-      </c>
-      <c r="C20" s="6">
-        <f>10 * SUM(C4:C19)</f>
+      <c r="B23" s="6">
+        <f>10 * SUM(B4:B22)</f>
+        <v>40</v>
+      </c>
+      <c r="C23" s="6">
+        <f>10 * SUM(C4:C22)</f>
         <v>10</v>
       </c>
-      <c r="D20" s="6">
-        <f>10 * SUM(D4:D19)</f>
+      <c r="D23" s="6">
+        <f>10 * SUM(D4:D22)</f>
         <v>40</v>
       </c>
-      <c r="E20" s="6">
-        <f>10 * SUM(E4:E19)</f>
+      <c r="E23" s="6">
+        <f>10 * SUM(E4:E22)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -732,8 +776,11 @@
     <row r="39" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="40" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="41" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="U9OFNnuH0TZ1prGHYAp8kx5c2jPW5gPl8fvGwoTN9EC0ZGqJbH2geZ7R6j3IRxwjDN5Q0LvbM21RU4dWVqrpXw==" saltValue="PeL1wkA58TwpjFKYxbrZaA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="VZJ6YEXFuDt+kaZyv0b4KgcX4EjfGI0EiNxop9iA7xoTAMIUAhjZDdtGFoc9Fcl04D7rf6OTMqfMa2VzI/pV3Q==" saltValue="yClV3ZqYtrKyeVmtCoTEdg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
   </mergeCells>

</xml_diff>